<commit_message>
Added Data Summary Columns
</commit_message>
<xml_diff>
--- a/output_excel.xlsx
+++ b/output_excel.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Attendance" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Attendance" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H152"/>
+  <dimension ref="A1:L152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,6 +490,26 @@
           <t>01/10/2024</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Total Attendance Marked</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Sum of Attendance</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Total Attendance Allowed</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Proxy</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -518,6 +538,18 @@
       <c r="H2" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I2" t="n">
+        <v>12</v>
+      </c>
+      <c r="J2" t="n">
+        <v>12</v>
+      </c>
+      <c r="K2" t="n">
+        <v>14</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -546,6 +578,18 @@
       <c r="H3" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I3" t="n">
+        <v>14</v>
+      </c>
+      <c r="J3" t="n">
+        <v>14</v>
+      </c>
+      <c r="K3" t="n">
+        <v>14</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -574,6 +618,18 @@
       <c r="H4" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I4" t="n">
+        <v>14</v>
+      </c>
+      <c r="J4" t="n">
+        <v>14</v>
+      </c>
+      <c r="K4" t="n">
+        <v>14</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -602,6 +658,18 @@
       <c r="H5" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="I5" t="n">
+        <v>12</v>
+      </c>
+      <c r="J5" t="n">
+        <v>12</v>
+      </c>
+      <c r="K5" t="n">
+        <v>14</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -630,6 +698,18 @@
       <c r="H6" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I6" t="n">
+        <v>13</v>
+      </c>
+      <c r="J6" t="n">
+        <v>13</v>
+      </c>
+      <c r="K6" t="n">
+        <v>14</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -658,6 +738,18 @@
       <c r="H7" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I7" t="n">
+        <v>13</v>
+      </c>
+      <c r="J7" t="n">
+        <v>12</v>
+      </c>
+      <c r="K7" t="n">
+        <v>14</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -686,6 +778,18 @@
       <c r="H8" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I8" t="n">
+        <v>12</v>
+      </c>
+      <c r="J8" t="n">
+        <v>10</v>
+      </c>
+      <c r="K8" t="n">
+        <v>14</v>
+      </c>
+      <c r="L8" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -714,6 +818,18 @@
       <c r="H9" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I9" t="n">
+        <v>12</v>
+      </c>
+      <c r="J9" t="n">
+        <v>12</v>
+      </c>
+      <c r="K9" t="n">
+        <v>14</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -742,6 +858,18 @@
       <c r="H10" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I10" t="n">
+        <v>14</v>
+      </c>
+      <c r="J10" t="n">
+        <v>14</v>
+      </c>
+      <c r="K10" t="n">
+        <v>14</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -770,6 +898,18 @@
       <c r="H11" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I11" t="n">
+        <v>14</v>
+      </c>
+      <c r="J11" t="n">
+        <v>14</v>
+      </c>
+      <c r="K11" t="n">
+        <v>14</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -798,6 +938,18 @@
       <c r="H12" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="I12" t="n">
+        <v>8</v>
+      </c>
+      <c r="J12" t="n">
+        <v>8</v>
+      </c>
+      <c r="K12" t="n">
+        <v>14</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -826,6 +978,18 @@
       <c r="H13" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I13" t="n">
+        <v>14</v>
+      </c>
+      <c r="J13" t="n">
+        <v>14</v>
+      </c>
+      <c r="K13" t="n">
+        <v>14</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -854,6 +1018,18 @@
       <c r="H14" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I14" t="n">
+        <v>12</v>
+      </c>
+      <c r="J14" t="n">
+        <v>12</v>
+      </c>
+      <c r="K14" t="n">
+        <v>14</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -882,6 +1058,18 @@
       <c r="H15" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="I15" t="n">
+        <v>10</v>
+      </c>
+      <c r="J15" t="n">
+        <v>10</v>
+      </c>
+      <c r="K15" t="n">
+        <v>14</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -910,6 +1098,18 @@
       <c r="H16" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I16" t="n">
+        <v>9</v>
+      </c>
+      <c r="J16" t="n">
+        <v>9</v>
+      </c>
+      <c r="K16" t="n">
+        <v>14</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -938,6 +1138,18 @@
       <c r="H17" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I17" t="n">
+        <v>14</v>
+      </c>
+      <c r="J17" t="n">
+        <v>14</v>
+      </c>
+      <c r="K17" t="n">
+        <v>14</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -966,6 +1178,18 @@
       <c r="H18" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>14</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -994,6 +1218,18 @@
       <c r="H19" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I19" t="n">
+        <v>8</v>
+      </c>
+      <c r="J19" t="n">
+        <v>8</v>
+      </c>
+      <c r="K19" t="n">
+        <v>14</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -1022,6 +1258,18 @@
       <c r="H20" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I20" t="n">
+        <v>10</v>
+      </c>
+      <c r="J20" t="n">
+        <v>10</v>
+      </c>
+      <c r="K20" t="n">
+        <v>14</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -1050,6 +1298,18 @@
       <c r="H21" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I21" t="n">
+        <v>13</v>
+      </c>
+      <c r="J21" t="n">
+        <v>12</v>
+      </c>
+      <c r="K21" t="n">
+        <v>14</v>
+      </c>
+      <c r="L21" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -1078,6 +1338,18 @@
       <c r="H22" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I22" t="n">
+        <v>14</v>
+      </c>
+      <c r="J22" t="n">
+        <v>14</v>
+      </c>
+      <c r="K22" t="n">
+        <v>14</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -1106,6 +1378,18 @@
       <c r="H23" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="I23" t="n">
+        <v>10</v>
+      </c>
+      <c r="J23" t="n">
+        <v>9</v>
+      </c>
+      <c r="K23" t="n">
+        <v>14</v>
+      </c>
+      <c r="L23" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -1134,6 +1418,18 @@
       <c r="H24" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I24" t="n">
+        <v>17</v>
+      </c>
+      <c r="J24" t="n">
+        <v>14</v>
+      </c>
+      <c r="K24" t="n">
+        <v>14</v>
+      </c>
+      <c r="L24" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -1162,6 +1458,18 @@
       <c r="H25" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I25" t="n">
+        <v>11</v>
+      </c>
+      <c r="J25" t="n">
+        <v>11</v>
+      </c>
+      <c r="K25" t="n">
+        <v>14</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -1190,6 +1498,18 @@
       <c r="H26" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I26" t="n">
+        <v>10</v>
+      </c>
+      <c r="J26" t="n">
+        <v>9</v>
+      </c>
+      <c r="K26" t="n">
+        <v>14</v>
+      </c>
+      <c r="L26" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -1218,6 +1538,18 @@
       <c r="H27" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I27" t="n">
+        <v>14</v>
+      </c>
+      <c r="J27" t="n">
+        <v>14</v>
+      </c>
+      <c r="K27" t="n">
+        <v>14</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -1246,6 +1578,18 @@
       <c r="H28" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I28" t="n">
+        <v>10</v>
+      </c>
+      <c r="J28" t="n">
+        <v>10</v>
+      </c>
+      <c r="K28" t="n">
+        <v>14</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
@@ -1274,6 +1618,18 @@
       <c r="H29" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I29" t="n">
+        <v>13</v>
+      </c>
+      <c r="J29" t="n">
+        <v>13</v>
+      </c>
+      <c r="K29" t="n">
+        <v>14</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
@@ -1302,6 +1658,18 @@
       <c r="H30" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I30" t="n">
+        <v>16</v>
+      </c>
+      <c r="J30" t="n">
+        <v>14</v>
+      </c>
+      <c r="K30" t="n">
+        <v>14</v>
+      </c>
+      <c r="L30" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
@@ -1330,6 +1698,18 @@
       <c r="H31" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I31" t="n">
+        <v>11</v>
+      </c>
+      <c r="J31" t="n">
+        <v>11</v>
+      </c>
+      <c r="K31" t="n">
+        <v>14</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
@@ -1358,6 +1738,18 @@
       <c r="H32" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I32" t="n">
+        <v>14</v>
+      </c>
+      <c r="J32" t="n">
+        <v>14</v>
+      </c>
+      <c r="K32" t="n">
+        <v>14</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
@@ -1386,6 +1778,18 @@
       <c r="H33" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I33" t="n">
+        <v>14</v>
+      </c>
+      <c r="J33" t="n">
+        <v>14</v>
+      </c>
+      <c r="K33" t="n">
+        <v>14</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
@@ -1414,6 +1818,18 @@
       <c r="H34" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I34" t="n">
+        <v>14</v>
+      </c>
+      <c r="J34" t="n">
+        <v>14</v>
+      </c>
+      <c r="K34" t="n">
+        <v>14</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
@@ -1442,6 +1858,18 @@
       <c r="H35" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I35" t="n">
+        <v>13</v>
+      </c>
+      <c r="J35" t="n">
+        <v>13</v>
+      </c>
+      <c r="K35" t="n">
+        <v>14</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
@@ -1470,6 +1898,18 @@
       <c r="H36" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I36" t="n">
+        <v>14</v>
+      </c>
+      <c r="J36" t="n">
+        <v>14</v>
+      </c>
+      <c r="K36" t="n">
+        <v>14</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
@@ -1498,6 +1938,18 @@
       <c r="H37" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I37" t="n">
+        <v>14</v>
+      </c>
+      <c r="J37" t="n">
+        <v>14</v>
+      </c>
+      <c r="K37" t="n">
+        <v>14</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
@@ -1526,6 +1978,18 @@
       <c r="H38" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I38" t="n">
+        <v>12</v>
+      </c>
+      <c r="J38" t="n">
+        <v>12</v>
+      </c>
+      <c r="K38" t="n">
+        <v>14</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
@@ -1554,6 +2018,18 @@
       <c r="H39" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I39" t="n">
+        <v>13</v>
+      </c>
+      <c r="J39" t="n">
+        <v>12</v>
+      </c>
+      <c r="K39" t="n">
+        <v>14</v>
+      </c>
+      <c r="L39" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
@@ -1582,6 +2058,18 @@
       <c r="H40" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I40" t="n">
+        <v>7</v>
+      </c>
+      <c r="J40" t="n">
+        <v>7</v>
+      </c>
+      <c r="K40" t="n">
+        <v>14</v>
+      </c>
+      <c r="L40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
@@ -1610,6 +2098,18 @@
       <c r="H41" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I41" t="n">
+        <v>12</v>
+      </c>
+      <c r="J41" t="n">
+        <v>12</v>
+      </c>
+      <c r="K41" t="n">
+        <v>14</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
@@ -1638,6 +2138,18 @@
       <c r="H42" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I42" t="n">
+        <v>12</v>
+      </c>
+      <c r="J42" t="n">
+        <v>12</v>
+      </c>
+      <c r="K42" t="n">
+        <v>14</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
@@ -1666,6 +2178,18 @@
       <c r="H43" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I43" t="n">
+        <v>5</v>
+      </c>
+      <c r="J43" t="n">
+        <v>5</v>
+      </c>
+      <c r="K43" t="n">
+        <v>14</v>
+      </c>
+      <c r="L43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
@@ -1694,6 +2218,18 @@
       <c r="H44" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I44" t="n">
+        <v>14</v>
+      </c>
+      <c r="J44" t="n">
+        <v>14</v>
+      </c>
+      <c r="K44" t="n">
+        <v>14</v>
+      </c>
+      <c r="L44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
@@ -1722,6 +2258,18 @@
       <c r="H45" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I45" t="n">
+        <v>14</v>
+      </c>
+      <c r="J45" t="n">
+        <v>14</v>
+      </c>
+      <c r="K45" t="n">
+        <v>14</v>
+      </c>
+      <c r="L45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
@@ -1750,6 +2298,18 @@
       <c r="H46" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I46" t="n">
+        <v>14</v>
+      </c>
+      <c r="J46" t="n">
+        <v>12</v>
+      </c>
+      <c r="K46" t="n">
+        <v>14</v>
+      </c>
+      <c r="L46" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
@@ -1778,6 +2338,18 @@
       <c r="H47" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I47" t="n">
+        <v>12</v>
+      </c>
+      <c r="J47" t="n">
+        <v>12</v>
+      </c>
+      <c r="K47" t="n">
+        <v>14</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
@@ -1806,6 +2378,18 @@
       <c r="H48" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I48" t="n">
+        <v>6</v>
+      </c>
+      <c r="J48" t="n">
+        <v>6</v>
+      </c>
+      <c r="K48" t="n">
+        <v>14</v>
+      </c>
+      <c r="L48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
@@ -1834,6 +2418,18 @@
       <c r="H49" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I49" t="n">
+        <v>4</v>
+      </c>
+      <c r="J49" t="n">
+        <v>4</v>
+      </c>
+      <c r="K49" t="n">
+        <v>14</v>
+      </c>
+      <c r="L49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
@@ -1862,6 +2458,18 @@
       <c r="H50" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K50" t="n">
+        <v>14</v>
+      </c>
+      <c r="L50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
@@ -1890,6 +2498,18 @@
       <c r="H51" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I51" t="n">
+        <v>12</v>
+      </c>
+      <c r="J51" t="n">
+        <v>12</v>
+      </c>
+      <c r="K51" t="n">
+        <v>14</v>
+      </c>
+      <c r="L51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
@@ -1918,6 +2538,18 @@
       <c r="H52" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I52" t="n">
+        <v>14</v>
+      </c>
+      <c r="J52" t="n">
+        <v>14</v>
+      </c>
+      <c r="K52" t="n">
+        <v>14</v>
+      </c>
+      <c r="L52" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
@@ -1946,6 +2578,18 @@
       <c r="H53" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I53" t="n">
+        <v>11</v>
+      </c>
+      <c r="J53" t="n">
+        <v>11</v>
+      </c>
+      <c r="K53" t="n">
+        <v>14</v>
+      </c>
+      <c r="L53" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
@@ -1974,6 +2618,18 @@
       <c r="H54" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I54" t="n">
+        <v>12</v>
+      </c>
+      <c r="J54" t="n">
+        <v>12</v>
+      </c>
+      <c r="K54" t="n">
+        <v>14</v>
+      </c>
+      <c r="L54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
@@ -2002,6 +2658,18 @@
       <c r="H55" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I55" t="n">
+        <v>8</v>
+      </c>
+      <c r="J55" t="n">
+        <v>6</v>
+      </c>
+      <c r="K55" t="n">
+        <v>14</v>
+      </c>
+      <c r="L55" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
@@ -2030,6 +2698,18 @@
       <c r="H56" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I56" t="n">
+        <v>12</v>
+      </c>
+      <c r="J56" t="n">
+        <v>12</v>
+      </c>
+      <c r="K56" t="n">
+        <v>14</v>
+      </c>
+      <c r="L56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
@@ -2058,6 +2738,18 @@
       <c r="H57" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I57" t="n">
+        <v>14</v>
+      </c>
+      <c r="J57" t="n">
+        <v>12</v>
+      </c>
+      <c r="K57" t="n">
+        <v>14</v>
+      </c>
+      <c r="L57" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
@@ -2086,6 +2778,18 @@
       <c r="H58" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I58" t="n">
+        <v>11</v>
+      </c>
+      <c r="J58" t="n">
+        <v>11</v>
+      </c>
+      <c r="K58" t="n">
+        <v>14</v>
+      </c>
+      <c r="L58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
@@ -2114,6 +2818,18 @@
       <c r="H59" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I59" t="n">
+        <v>12</v>
+      </c>
+      <c r="J59" t="n">
+        <v>12</v>
+      </c>
+      <c r="K59" t="n">
+        <v>14</v>
+      </c>
+      <c r="L59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
@@ -2142,6 +2858,18 @@
       <c r="H60" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I60" t="n">
+        <v>10</v>
+      </c>
+      <c r="J60" t="n">
+        <v>10</v>
+      </c>
+      <c r="K60" t="n">
+        <v>14</v>
+      </c>
+      <c r="L60" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
@@ -2170,6 +2898,18 @@
       <c r="H61" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I61" t="n">
+        <v>14</v>
+      </c>
+      <c r="J61" t="n">
+        <v>14</v>
+      </c>
+      <c r="K61" t="n">
+        <v>14</v>
+      </c>
+      <c r="L61" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
@@ -2198,6 +2938,18 @@
       <c r="H62" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="I62" t="n">
+        <v>10</v>
+      </c>
+      <c r="J62" t="n">
+        <v>10</v>
+      </c>
+      <c r="K62" t="n">
+        <v>14</v>
+      </c>
+      <c r="L62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
@@ -2226,6 +2978,18 @@
       <c r="H63" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I63" t="n">
+        <v>11</v>
+      </c>
+      <c r="J63" t="n">
+        <v>11</v>
+      </c>
+      <c r="K63" t="n">
+        <v>14</v>
+      </c>
+      <c r="L63" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
@@ -2254,6 +3018,18 @@
       <c r="H64" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I64" t="n">
+        <v>15</v>
+      </c>
+      <c r="J64" t="n">
+        <v>14</v>
+      </c>
+      <c r="K64" t="n">
+        <v>14</v>
+      </c>
+      <c r="L64" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
@@ -2282,6 +3058,18 @@
       <c r="H65" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I65" t="n">
+        <v>8</v>
+      </c>
+      <c r="J65" t="n">
+        <v>8</v>
+      </c>
+      <c r="K65" t="n">
+        <v>14</v>
+      </c>
+      <c r="L65" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
@@ -2310,6 +3098,18 @@
       <c r="H66" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I66" t="n">
+        <v>12</v>
+      </c>
+      <c r="J66" t="n">
+        <v>12</v>
+      </c>
+      <c r="K66" t="n">
+        <v>14</v>
+      </c>
+      <c r="L66" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
@@ -2338,6 +3138,18 @@
       <c r="H67" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I67" t="n">
+        <v>8</v>
+      </c>
+      <c r="J67" t="n">
+        <v>8</v>
+      </c>
+      <c r="K67" t="n">
+        <v>14</v>
+      </c>
+      <c r="L67" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
@@ -2366,6 +3178,18 @@
       <c r="H68" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I68" t="n">
+        <v>13</v>
+      </c>
+      <c r="J68" t="n">
+        <v>12</v>
+      </c>
+      <c r="K68" t="n">
+        <v>14</v>
+      </c>
+      <c r="L68" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
@@ -2394,6 +3218,18 @@
       <c r="H69" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="I69" t="n">
+        <v>13</v>
+      </c>
+      <c r="J69" t="n">
+        <v>13</v>
+      </c>
+      <c r="K69" t="n">
+        <v>14</v>
+      </c>
+      <c r="L69" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
@@ -2422,6 +3258,18 @@
       <c r="H70" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I70" t="n">
+        <v>9</v>
+      </c>
+      <c r="J70" t="n">
+        <v>8</v>
+      </c>
+      <c r="K70" t="n">
+        <v>14</v>
+      </c>
+      <c r="L70" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
@@ -2450,6 +3298,18 @@
       <c r="H71" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I71" t="n">
+        <v>14</v>
+      </c>
+      <c r="J71" t="n">
+        <v>14</v>
+      </c>
+      <c r="K71" t="n">
+        <v>14</v>
+      </c>
+      <c r="L71" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
@@ -2478,6 +3338,18 @@
       <c r="H72" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I72" t="n">
+        <v>12</v>
+      </c>
+      <c r="J72" t="n">
+        <v>12</v>
+      </c>
+      <c r="K72" t="n">
+        <v>14</v>
+      </c>
+      <c r="L72" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
@@ -2506,6 +3378,18 @@
       <c r="H73" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="I73" t="n">
+        <v>13</v>
+      </c>
+      <c r="J73" t="n">
+        <v>13</v>
+      </c>
+      <c r="K73" t="n">
+        <v>14</v>
+      </c>
+      <c r="L73" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
@@ -2534,6 +3418,18 @@
       <c r="H74" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I74" t="n">
+        <v>7</v>
+      </c>
+      <c r="J74" t="n">
+        <v>7</v>
+      </c>
+      <c r="K74" t="n">
+        <v>14</v>
+      </c>
+      <c r="L74" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
@@ -2562,6 +3458,18 @@
       <c r="H75" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="I75" t="n">
+        <v>8</v>
+      </c>
+      <c r="J75" t="n">
+        <v>8</v>
+      </c>
+      <c r="K75" t="n">
+        <v>14</v>
+      </c>
+      <c r="L75" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
@@ -2590,6 +3498,18 @@
       <c r="H76" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I76" t="n">
+        <v>15</v>
+      </c>
+      <c r="J76" t="n">
+        <v>14</v>
+      </c>
+      <c r="K76" t="n">
+        <v>14</v>
+      </c>
+      <c r="L76" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
@@ -2618,6 +3538,18 @@
       <c r="H77" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I77" t="n">
+        <v>14</v>
+      </c>
+      <c r="J77" t="n">
+        <v>14</v>
+      </c>
+      <c r="K77" t="n">
+        <v>14</v>
+      </c>
+      <c r="L77" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
@@ -2646,6 +3578,18 @@
       <c r="H78" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I78" t="n">
+        <v>13</v>
+      </c>
+      <c r="J78" t="n">
+        <v>12</v>
+      </c>
+      <c r="K78" t="n">
+        <v>14</v>
+      </c>
+      <c r="L78" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
@@ -2674,6 +3618,18 @@
       <c r="H79" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I79" t="n">
+        <v>12</v>
+      </c>
+      <c r="J79" t="n">
+        <v>12</v>
+      </c>
+      <c r="K79" t="n">
+        <v>14</v>
+      </c>
+      <c r="L79" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
@@ -2702,6 +3658,18 @@
       <c r="H80" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I80" t="n">
+        <v>14</v>
+      </c>
+      <c r="J80" t="n">
+        <v>10</v>
+      </c>
+      <c r="K80" t="n">
+        <v>14</v>
+      </c>
+      <c r="L80" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
@@ -2730,6 +3698,18 @@
       <c r="H81" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I81" t="n">
+        <v>14</v>
+      </c>
+      <c r="J81" t="n">
+        <v>13</v>
+      </c>
+      <c r="K81" t="n">
+        <v>14</v>
+      </c>
+      <c r="L81" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
@@ -2758,6 +3738,18 @@
       <c r="H82" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I82" t="n">
+        <v>10</v>
+      </c>
+      <c r="J82" t="n">
+        <v>10</v>
+      </c>
+      <c r="K82" t="n">
+        <v>14</v>
+      </c>
+      <c r="L82" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
@@ -2786,6 +3778,18 @@
       <c r="H83" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I83" t="n">
+        <v>10</v>
+      </c>
+      <c r="J83" t="n">
+        <v>10</v>
+      </c>
+      <c r="K83" t="n">
+        <v>14</v>
+      </c>
+      <c r="L83" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
@@ -2814,6 +3818,18 @@
       <c r="H84" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I84" t="n">
+        <v>10</v>
+      </c>
+      <c r="J84" t="n">
+        <v>10</v>
+      </c>
+      <c r="K84" t="n">
+        <v>14</v>
+      </c>
+      <c r="L84" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
@@ -2842,6 +3858,18 @@
       <c r="H85" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I85" t="n">
+        <v>11</v>
+      </c>
+      <c r="J85" t="n">
+        <v>11</v>
+      </c>
+      <c r="K85" t="n">
+        <v>14</v>
+      </c>
+      <c r="L85" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
@@ -2870,6 +3898,18 @@
       <c r="H86" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I86" t="n">
+        <v>12</v>
+      </c>
+      <c r="J86" t="n">
+        <v>10</v>
+      </c>
+      <c r="K86" t="n">
+        <v>14</v>
+      </c>
+      <c r="L86" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
@@ -2898,6 +3938,18 @@
       <c r="H87" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I87" t="n">
+        <v>8</v>
+      </c>
+      <c r="J87" t="n">
+        <v>8</v>
+      </c>
+      <c r="K87" t="n">
+        <v>14</v>
+      </c>
+      <c r="L87" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
@@ -2926,6 +3978,18 @@
       <c r="H88" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I88" t="n">
+        <v>10</v>
+      </c>
+      <c r="J88" t="n">
+        <v>10</v>
+      </c>
+      <c r="K88" t="n">
+        <v>14</v>
+      </c>
+      <c r="L88" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
@@ -2954,6 +4018,18 @@
       <c r="H89" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I89" t="n">
+        <v>9</v>
+      </c>
+      <c r="J89" t="n">
+        <v>9</v>
+      </c>
+      <c r="K89" t="n">
+        <v>14</v>
+      </c>
+      <c r="L89" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
@@ -2982,6 +4058,18 @@
       <c r="H90" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I90" t="n">
+        <v>8</v>
+      </c>
+      <c r="J90" t="n">
+        <v>8</v>
+      </c>
+      <c r="K90" t="n">
+        <v>14</v>
+      </c>
+      <c r="L90" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
@@ -3010,6 +4098,18 @@
       <c r="H91" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I91" t="n">
+        <v>15</v>
+      </c>
+      <c r="J91" t="n">
+        <v>14</v>
+      </c>
+      <c r="K91" t="n">
+        <v>14</v>
+      </c>
+      <c r="L91" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
@@ -3038,6 +4138,18 @@
       <c r="H92" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I92" t="n">
+        <v>12</v>
+      </c>
+      <c r="J92" t="n">
+        <v>12</v>
+      </c>
+      <c r="K92" t="n">
+        <v>14</v>
+      </c>
+      <c r="L92" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
@@ -3066,6 +4178,18 @@
       <c r="H93" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I93" t="n">
+        <v>0</v>
+      </c>
+      <c r="J93" t="n">
+        <v>0</v>
+      </c>
+      <c r="K93" t="n">
+        <v>14</v>
+      </c>
+      <c r="L93" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
@@ -3094,6 +4218,18 @@
       <c r="H94" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I94" t="n">
+        <v>14</v>
+      </c>
+      <c r="J94" t="n">
+        <v>14</v>
+      </c>
+      <c r="K94" t="n">
+        <v>14</v>
+      </c>
+      <c r="L94" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
@@ -3122,6 +4258,18 @@
       <c r="H95" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I95" t="n">
+        <v>10</v>
+      </c>
+      <c r="J95" t="n">
+        <v>10</v>
+      </c>
+      <c r="K95" t="n">
+        <v>14</v>
+      </c>
+      <c r="L95" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
@@ -3150,6 +4298,18 @@
       <c r="H96" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I96" t="n">
+        <v>9</v>
+      </c>
+      <c r="J96" t="n">
+        <v>9</v>
+      </c>
+      <c r="K96" t="n">
+        <v>14</v>
+      </c>
+      <c r="L96" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
@@ -3178,6 +4338,18 @@
       <c r="H97" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I97" t="n">
+        <v>8</v>
+      </c>
+      <c r="J97" t="n">
+        <v>8</v>
+      </c>
+      <c r="K97" t="n">
+        <v>14</v>
+      </c>
+      <c r="L97" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
@@ -3206,6 +4378,18 @@
       <c r="H98" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I98" t="n">
+        <v>12</v>
+      </c>
+      <c r="J98" t="n">
+        <v>12</v>
+      </c>
+      <c r="K98" t="n">
+        <v>14</v>
+      </c>
+      <c r="L98" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
@@ -3234,6 +4418,18 @@
       <c r="H99" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I99" t="n">
+        <v>12</v>
+      </c>
+      <c r="J99" t="n">
+        <v>12</v>
+      </c>
+      <c r="K99" t="n">
+        <v>14</v>
+      </c>
+      <c r="L99" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
@@ -3262,6 +4458,18 @@
       <c r="H100" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I100" t="n">
+        <v>7</v>
+      </c>
+      <c r="J100" t="n">
+        <v>7</v>
+      </c>
+      <c r="K100" t="n">
+        <v>14</v>
+      </c>
+      <c r="L100" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
@@ -3290,6 +4498,18 @@
       <c r="H101" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I101" t="n">
+        <v>15</v>
+      </c>
+      <c r="J101" t="n">
+        <v>14</v>
+      </c>
+      <c r="K101" t="n">
+        <v>14</v>
+      </c>
+      <c r="L101" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
@@ -3318,6 +4538,18 @@
       <c r="H102" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I102" t="n">
+        <v>13</v>
+      </c>
+      <c r="J102" t="n">
+        <v>10</v>
+      </c>
+      <c r="K102" t="n">
+        <v>14</v>
+      </c>
+      <c r="L102" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
@@ -3346,6 +4578,18 @@
       <c r="H103" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I103" t="n">
+        <v>14</v>
+      </c>
+      <c r="J103" t="n">
+        <v>14</v>
+      </c>
+      <c r="K103" t="n">
+        <v>14</v>
+      </c>
+      <c r="L103" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
@@ -3374,6 +4618,18 @@
       <c r="H104" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I104" t="n">
+        <v>14</v>
+      </c>
+      <c r="J104" t="n">
+        <v>14</v>
+      </c>
+      <c r="K104" t="n">
+        <v>14</v>
+      </c>
+      <c r="L104" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
@@ -3402,6 +4658,18 @@
       <c r="H105" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I105" t="n">
+        <v>13</v>
+      </c>
+      <c r="J105" t="n">
+        <v>13</v>
+      </c>
+      <c r="K105" t="n">
+        <v>14</v>
+      </c>
+      <c r="L105" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
@@ -3430,6 +4698,18 @@
       <c r="H106" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I106" t="n">
+        <v>14</v>
+      </c>
+      <c r="J106" t="n">
+        <v>14</v>
+      </c>
+      <c r="K106" t="n">
+        <v>14</v>
+      </c>
+      <c r="L106" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
@@ -3458,6 +4738,18 @@
       <c r="H107" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I107" t="n">
+        <v>14</v>
+      </c>
+      <c r="J107" t="n">
+        <v>14</v>
+      </c>
+      <c r="K107" t="n">
+        <v>14</v>
+      </c>
+      <c r="L107" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
@@ -3486,6 +4778,18 @@
       <c r="H108" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I108" t="n">
+        <v>8</v>
+      </c>
+      <c r="J108" t="n">
+        <v>8</v>
+      </c>
+      <c r="K108" t="n">
+        <v>14</v>
+      </c>
+      <c r="L108" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
@@ -3514,6 +4818,18 @@
       <c r="H109" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I109" t="n">
+        <v>14</v>
+      </c>
+      <c r="J109" t="n">
+        <v>14</v>
+      </c>
+      <c r="K109" t="n">
+        <v>14</v>
+      </c>
+      <c r="L109" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
@@ -3542,6 +4858,18 @@
       <c r="H110" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I110" t="n">
+        <v>12</v>
+      </c>
+      <c r="J110" t="n">
+        <v>12</v>
+      </c>
+      <c r="K110" t="n">
+        <v>14</v>
+      </c>
+      <c r="L110" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
@@ -3570,6 +4898,18 @@
       <c r="H111" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="I111" t="n">
+        <v>9</v>
+      </c>
+      <c r="J111" t="n">
+        <v>9</v>
+      </c>
+      <c r="K111" t="n">
+        <v>14</v>
+      </c>
+      <c r="L111" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
@@ -3598,6 +4938,18 @@
       <c r="H112" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="I112" t="n">
+        <v>8</v>
+      </c>
+      <c r="J112" t="n">
+        <v>8</v>
+      </c>
+      <c r="K112" t="n">
+        <v>14</v>
+      </c>
+      <c r="L112" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
@@ -3626,6 +4978,18 @@
       <c r="H113" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I113" t="n">
+        <v>14</v>
+      </c>
+      <c r="J113" t="n">
+        <v>14</v>
+      </c>
+      <c r="K113" t="n">
+        <v>14</v>
+      </c>
+      <c r="L113" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
@@ -3654,6 +5018,18 @@
       <c r="H114" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I114" t="n">
+        <v>15</v>
+      </c>
+      <c r="J114" t="n">
+        <v>12</v>
+      </c>
+      <c r="K114" t="n">
+        <v>14</v>
+      </c>
+      <c r="L114" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
@@ -3682,6 +5058,18 @@
       <c r="H115" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I115" t="n">
+        <v>13</v>
+      </c>
+      <c r="J115" t="n">
+        <v>13</v>
+      </c>
+      <c r="K115" t="n">
+        <v>14</v>
+      </c>
+      <c r="L115" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
@@ -3710,6 +5098,18 @@
       <c r="H116" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I116" t="n">
+        <v>14</v>
+      </c>
+      <c r="J116" t="n">
+        <v>14</v>
+      </c>
+      <c r="K116" t="n">
+        <v>14</v>
+      </c>
+      <c r="L116" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
@@ -3738,6 +5138,18 @@
       <c r="H117" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I117" t="n">
+        <v>12</v>
+      </c>
+      <c r="J117" t="n">
+        <v>10</v>
+      </c>
+      <c r="K117" t="n">
+        <v>14</v>
+      </c>
+      <c r="L117" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
@@ -3766,6 +5178,18 @@
       <c r="H118" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="I118" t="n">
+        <v>12</v>
+      </c>
+      <c r="J118" t="n">
+        <v>12</v>
+      </c>
+      <c r="K118" t="n">
+        <v>14</v>
+      </c>
+      <c r="L118" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
@@ -3794,6 +5218,18 @@
       <c r="H119" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I119" t="n">
+        <v>14</v>
+      </c>
+      <c r="J119" t="n">
+        <v>14</v>
+      </c>
+      <c r="K119" t="n">
+        <v>14</v>
+      </c>
+      <c r="L119" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
@@ -3822,6 +5258,18 @@
       <c r="H120" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I120" t="n">
+        <v>12</v>
+      </c>
+      <c r="J120" t="n">
+        <v>12</v>
+      </c>
+      <c r="K120" t="n">
+        <v>14</v>
+      </c>
+      <c r="L120" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
@@ -3850,6 +5298,18 @@
       <c r="H121" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I121" t="n">
+        <v>6</v>
+      </c>
+      <c r="J121" t="n">
+        <v>5</v>
+      </c>
+      <c r="K121" t="n">
+        <v>14</v>
+      </c>
+      <c r="L121" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
@@ -3878,6 +5338,18 @@
       <c r="H122" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I122" t="n">
+        <v>13</v>
+      </c>
+      <c r="J122" t="n">
+        <v>12</v>
+      </c>
+      <c r="K122" t="n">
+        <v>14</v>
+      </c>
+      <c r="L122" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
@@ -3906,6 +5378,18 @@
       <c r="H123" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I123" t="n">
+        <v>14</v>
+      </c>
+      <c r="J123" t="n">
+        <v>13</v>
+      </c>
+      <c r="K123" t="n">
+        <v>14</v>
+      </c>
+      <c r="L123" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
@@ -3934,6 +5418,18 @@
       <c r="H124" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I124" t="n">
+        <v>10</v>
+      </c>
+      <c r="J124" t="n">
+        <v>10</v>
+      </c>
+      <c r="K124" t="n">
+        <v>14</v>
+      </c>
+      <c r="L124" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="inlineStr">
@@ -3962,6 +5458,18 @@
       <c r="H125" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I125" t="n">
+        <v>12</v>
+      </c>
+      <c r="J125" t="n">
+        <v>12</v>
+      </c>
+      <c r="K125" t="n">
+        <v>14</v>
+      </c>
+      <c r="L125" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="inlineStr">
@@ -3990,6 +5498,18 @@
       <c r="H126" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I126" t="n">
+        <v>12</v>
+      </c>
+      <c r="J126" t="n">
+        <v>12</v>
+      </c>
+      <c r="K126" t="n">
+        <v>14</v>
+      </c>
+      <c r="L126" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
@@ -4018,6 +5538,18 @@
       <c r="H127" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I127" t="n">
+        <v>14</v>
+      </c>
+      <c r="J127" t="n">
+        <v>14</v>
+      </c>
+      <c r="K127" t="n">
+        <v>14</v>
+      </c>
+      <c r="L127" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
@@ -4046,6 +5578,18 @@
       <c r="H128" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I128" t="n">
+        <v>6</v>
+      </c>
+      <c r="J128" t="n">
+        <v>6</v>
+      </c>
+      <c r="K128" t="n">
+        <v>14</v>
+      </c>
+      <c r="L128" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
@@ -4074,6 +5618,18 @@
       <c r="H129" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I129" t="n">
+        <v>14</v>
+      </c>
+      <c r="J129" t="n">
+        <v>14</v>
+      </c>
+      <c r="K129" t="n">
+        <v>14</v>
+      </c>
+      <c r="L129" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="inlineStr">
@@ -4102,6 +5658,18 @@
       <c r="H130" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I130" t="n">
+        <v>16</v>
+      </c>
+      <c r="J130" t="n">
+        <v>14</v>
+      </c>
+      <c r="K130" t="n">
+        <v>14</v>
+      </c>
+      <c r="L130" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="inlineStr">
@@ -4130,6 +5698,18 @@
       <c r="H131" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I131" t="n">
+        <v>14</v>
+      </c>
+      <c r="J131" t="n">
+        <v>14</v>
+      </c>
+      <c r="K131" t="n">
+        <v>14</v>
+      </c>
+      <c r="L131" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
@@ -4158,6 +5738,18 @@
       <c r="H132" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I132" t="n">
+        <v>8</v>
+      </c>
+      <c r="J132" t="n">
+        <v>8</v>
+      </c>
+      <c r="K132" t="n">
+        <v>14</v>
+      </c>
+      <c r="L132" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
@@ -4186,6 +5778,18 @@
       <c r="H133" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I133" t="n">
+        <v>13</v>
+      </c>
+      <c r="J133" t="n">
+        <v>12</v>
+      </c>
+      <c r="K133" t="n">
+        <v>14</v>
+      </c>
+      <c r="L133" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="inlineStr">
@@ -4214,6 +5818,18 @@
       <c r="H134" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I134" t="n">
+        <v>14</v>
+      </c>
+      <c r="J134" t="n">
+        <v>14</v>
+      </c>
+      <c r="K134" t="n">
+        <v>14</v>
+      </c>
+      <c r="L134" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="inlineStr">
@@ -4242,6 +5858,18 @@
       <c r="H135" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I135" t="n">
+        <v>14</v>
+      </c>
+      <c r="J135" t="n">
+        <v>13</v>
+      </c>
+      <c r="K135" t="n">
+        <v>14</v>
+      </c>
+      <c r="L135" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="inlineStr">
@@ -4270,6 +5898,18 @@
       <c r="H136" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I136" t="n">
+        <v>14</v>
+      </c>
+      <c r="J136" t="n">
+        <v>14</v>
+      </c>
+      <c r="K136" t="n">
+        <v>14</v>
+      </c>
+      <c r="L136" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
@@ -4298,6 +5938,18 @@
       <c r="H137" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I137" t="n">
+        <v>14</v>
+      </c>
+      <c r="J137" t="n">
+        <v>14</v>
+      </c>
+      <c r="K137" t="n">
+        <v>14</v>
+      </c>
+      <c r="L137" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="inlineStr">
@@ -4326,6 +5978,18 @@
       <c r="H138" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="I138" t="n">
+        <v>8</v>
+      </c>
+      <c r="J138" t="n">
+        <v>8</v>
+      </c>
+      <c r="K138" t="n">
+        <v>14</v>
+      </c>
+      <c r="L138" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
@@ -4354,6 +6018,18 @@
       <c r="H139" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I139" t="n">
+        <v>10</v>
+      </c>
+      <c r="J139" t="n">
+        <v>10</v>
+      </c>
+      <c r="K139" t="n">
+        <v>14</v>
+      </c>
+      <c r="L139" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="inlineStr">
@@ -4382,6 +6058,18 @@
       <c r="H140" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I140" t="n">
+        <v>13</v>
+      </c>
+      <c r="J140" t="n">
+        <v>13</v>
+      </c>
+      <c r="K140" t="n">
+        <v>14</v>
+      </c>
+      <c r="L140" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="inlineStr">
@@ -4410,6 +6098,18 @@
       <c r="H141" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I141" t="n">
+        <v>12</v>
+      </c>
+      <c r="J141" t="n">
+        <v>11</v>
+      </c>
+      <c r="K141" t="n">
+        <v>14</v>
+      </c>
+      <c r="L141" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
@@ -4438,6 +6138,18 @@
       <c r="H142" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="I142" t="n">
+        <v>10</v>
+      </c>
+      <c r="J142" t="n">
+        <v>9</v>
+      </c>
+      <c r="K142" t="n">
+        <v>14</v>
+      </c>
+      <c r="L142" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="inlineStr">
@@ -4466,6 +6178,18 @@
       <c r="H143" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I143" t="n">
+        <v>13</v>
+      </c>
+      <c r="J143" t="n">
+        <v>12</v>
+      </c>
+      <c r="K143" t="n">
+        <v>14</v>
+      </c>
+      <c r="L143" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="inlineStr">
@@ -4494,6 +6218,18 @@
       <c r="H144" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I144" t="n">
+        <v>14</v>
+      </c>
+      <c r="J144" t="n">
+        <v>14</v>
+      </c>
+      <c r="K144" t="n">
+        <v>14</v>
+      </c>
+      <c r="L144" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="inlineStr">
@@ -4522,6 +6258,18 @@
       <c r="H145" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I145" t="n">
+        <v>13</v>
+      </c>
+      <c r="J145" t="n">
+        <v>13</v>
+      </c>
+      <c r="K145" t="n">
+        <v>14</v>
+      </c>
+      <c r="L145" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="inlineStr">
@@ -4550,6 +6298,18 @@
       <c r="H146" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I146" t="n">
+        <v>14</v>
+      </c>
+      <c r="J146" t="n">
+        <v>14</v>
+      </c>
+      <c r="K146" t="n">
+        <v>14</v>
+      </c>
+      <c r="L146" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="inlineStr">
@@ -4578,6 +6338,18 @@
       <c r="H147" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I147" t="n">
+        <v>14</v>
+      </c>
+      <c r="J147" t="n">
+        <v>14</v>
+      </c>
+      <c r="K147" t="n">
+        <v>14</v>
+      </c>
+      <c r="L147" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="inlineStr">
@@ -4606,6 +6378,18 @@
       <c r="H148" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I148" t="n">
+        <v>15</v>
+      </c>
+      <c r="J148" t="n">
+        <v>14</v>
+      </c>
+      <c r="K148" t="n">
+        <v>14</v>
+      </c>
+      <c r="L148" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
@@ -4634,6 +6418,18 @@
       <c r="H149" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I149" t="n">
+        <v>13</v>
+      </c>
+      <c r="J149" t="n">
+        <v>12</v>
+      </c>
+      <c r="K149" t="n">
+        <v>14</v>
+      </c>
+      <c r="L149" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="inlineStr">
@@ -4662,6 +6458,18 @@
       <c r="H150" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I150" t="n">
+        <v>15</v>
+      </c>
+      <c r="J150" t="n">
+        <v>14</v>
+      </c>
+      <c r="K150" t="n">
+        <v>14</v>
+      </c>
+      <c r="L150" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="inlineStr">
@@ -4690,6 +6498,18 @@
       <c r="H151" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="I151" t="n">
+        <v>8</v>
+      </c>
+      <c r="J151" t="n">
+        <v>8</v>
+      </c>
+      <c r="K151" t="n">
+        <v>14</v>
+      </c>
+      <c r="L151" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="inlineStr">
@@ -4717,6 +6537,18 @@
       </c>
       <c r="H152" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="I152" t="n">
+        <v>17</v>
+      </c>
+      <c r="J152" t="n">
+        <v>14</v>
+      </c>
+      <c r="K152" t="n">
+        <v>14</v>
+      </c>
+      <c r="L152" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>